<commit_message>
MTP049 COP rows delivered
</commit_message>
<xml_diff>
--- a/observations/region_priorities.xlsx
+++ b/observations/region_priorities.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEA0F28-D701-4145-A91D-41136D174AE2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650AC336-82A6-4767-9F50-DF03D42EC597}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2385" yWindow="1800" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -90,14 +90,14 @@
     <t>Normal priority (~1 in 3 overflights)</t>
   </si>
   <si>
-    <t>New Priority</t>
+    <t>New Priorities MTP049 onwards</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +107,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -160,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -171,6 +180,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -456,7 +468,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,7 +478,7 @@
     <col min="3" max="3" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -476,9 +488,7 @@
       <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -577,6 +587,11 @@
       </c>
       <c r="C10" s="2" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>